<commit_message>
revisi alert tgl produksi dan revisi manager gbj
</commit_message>
<xml_diff>
--- a/public/upload/noseri/Template Noseri(1).xlsx
+++ b/public/upload/noseri/Template Noseri(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Noseri" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="298">
   <si>
     <t>No</t>
   </si>
@@ -907,16 +907,13 @@
     <t xml:space="preserve">ZTP80AS-UPGRADE </t>
   </si>
   <si>
-    <t>TR10223A00134</t>
-  </si>
-  <si>
-    <t>TR10223A00231</t>
-  </si>
-  <si>
-    <t>TR10223A00328</t>
-  </si>
-  <si>
-    <t>TR10223A00442</t>
+    <t>AS65466363</t>
+  </si>
+  <si>
+    <t>AS65466362</t>
+  </si>
+  <si>
+    <t>AS65466361</t>
   </si>
 </sst>
 </file>
@@ -1267,15 +1264,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1290,47 +1287,27 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1358,9 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>